<commit_message>
DMS: KpiProductGrouping Add ExportTemplate
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_Product_Grouping_Report.xlsx
+++ b/DMS/Templates/Kpi_Product_Grouping_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2BCA32-DFAF-4DB0-8AC2-CB1E17090CF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B373CDD8-2DDF-4871-BFAE-FF9B25DA865A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,61 +48,61 @@
     <t>Số đại lý hiện diện</t>
   </si>
   <si>
-    <t>Kỳ KPI: Tháng 4 - Năm: 2021</t>
-  </si>
-  <si>
-    <t>00000014</t>
-  </si>
-  <si>
-    <t>Đèn LED Gắn tường GT12 5W 6500K</t>
-  </si>
-  <si>
-    <t>00000024</t>
-  </si>
-  <si>
-    <t>Đèn LED nổi trần D400 DNT 01L/30W-4000K</t>
-  </si>
-  <si>
-    <t>00000005</t>
-  </si>
-  <si>
-    <t>Đèn LED Gắn tường GT04 HG/5W 6500K</t>
-  </si>
-  <si>
     <t>BÁO CÁO KPI NHÓM SẢN PHẨM</t>
   </si>
   <si>
-    <t>Loại KPI: KPI nhóm sản phẩm mới</t>
-  </si>
-  <si>
     <t>Mã nhóm sản phẩm</t>
   </si>
   <si>
     <t>Tên nhóm sản phẩm</t>
   </si>
   <si>
-    <t>Truyền thống vùng 1</t>
-  </si>
-  <si>
-    <t>Truyền thống vùng 2</t>
-  </si>
-  <si>
     <t>Mã nhân viên</t>
   </si>
   <si>
     <t>Tên nhân viên</t>
   </si>
   <si>
-    <t>Tv01.NhungLT</t>
-  </si>
-  <si>
-    <t>Lê Thị Nhung</t>
-  </si>
-  <si>
-    <t>TV02.Anh</t>
-  </si>
-  <si>
-    <t>Lê Thị Anh</t>
+    <t>Kỳ KPI: {{KpiPeriod}} - Năm: {{KpiYear}}</t>
+  </si>
+  <si>
+    <t>Loại KPI: {{KpiProductGroupingType}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.OrganizationName}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.STT}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.Username}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.DisplayName}}</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.ProductGroupingCode}}</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.ProductGroupingName}}</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectRevenuePlanned}}</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectRevenue}}</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectRevenueRatio}}</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectStorePlanned}}</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectStore}}</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectStoreRatio}}</t>
   </si>
 </sst>
 </file>
@@ -170,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -234,6 +234,15 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -247,6 +256,15 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -260,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -276,30 +294,6 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -321,6 +315,33 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,125 +623,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
-    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+    <row r="4" spans="1:14" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="17" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="17" t="s">
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
       <c r="I8" s="3" t="s">
         <v>2</v>
       </c>
@@ -730,143 +763,87 @@
       <c r="K8" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="L8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="17"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>1</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="H10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="L10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="5">
-        <v>300000000</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="5">
-        <v>400000000000</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>2</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="M10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="N10" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="5">
-        <v>200000</v>
-      </c>
-      <c r="G13" s="5">
-        <v>24200000</v>
-      </c>
-      <c r="H13" s="6">
-        <v>12100</v>
-      </c>
-      <c r="I13" s="5">
-        <v>10</v>
-      </c>
-      <c r="J13" s="5">
-        <v>1</v>
-      </c>
-      <c r="K13" s="6">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="F7:H7"/>
+  <mergeCells count="13">
+    <mergeCell ref="A9:N9"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
DMS: Fix List KpiProductGroupingReport
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_Product_Grouping_Report.xlsx
+++ b/DMS/Templates/Kpi_Product_Grouping_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B373CDD8-2DDF-4871-BFAE-FF9B25DA865A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52BBF95-7F8F-43B8-9DA4-ECA166396556}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,34 +75,34 @@
     <t>{{KpiProductGroupingReports.SaleEmployees.STT}}</t>
   </si>
   <si>
-    <t>{{KpiProductGroupingReports.SaleEmployees.Username}}</t>
-  </si>
-  <si>
     <t>{{KpiProductGroupingReports.SaleEmployees.DisplayName}}</t>
   </si>
   <si>
-    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.ProductGroupingCode}}</t>
-  </si>
-  <si>
-    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.ProductGroupingName}}</t>
-  </si>
-  <si>
-    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectRevenuePlanned}}</t>
-  </si>
-  <si>
-    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectRevenue}}</t>
-  </si>
-  <si>
-    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectRevenueRatio}}</t>
-  </si>
-  <si>
-    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectStorePlanned}}</t>
-  </si>
-  <si>
-    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectStore}}</t>
-  </si>
-  <si>
-    <t>{{ReportSalesOrderByEmployeeAndItems.SaleEmployees.Contents.IndirectStoreRatio}}</t>
+    <t>{{KpiProductGroupingReports.SaleEmployees.UserName}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.Contents.ProductGroupingCode}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.Contents.ProductGroupingName}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.Contents.IndirectRevenuePlanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.Contents.IndirectRevenue}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.Contents.IndirectRevenueRatio}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.Contents.IndirectStorePlanned}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.Contents.IndirectStore}}</t>
+  </si>
+  <si>
+    <t>{{KpiProductGroupingReports.SaleEmployees.Contents.IndirectStoreRatio}}</t>
   </si>
 </sst>
 </file>
@@ -294,8 +294,11 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -337,11 +340,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,17 +629,17 @@
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
     <col min="8" max="8" width="39.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" style="1" customWidth="1"/>
@@ -652,50 +652,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="4" spans="1:14" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -704,56 +704,56 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="14" t="s">
+      <c r="H5" s="23"/>
+      <c r="I5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="18" t="s">
+      <c r="D7" s="20"/>
+      <c r="E7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="20"/>
+      <c r="G7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="9" t="s">
+      <c r="J7" s="11"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
       <c r="I8" s="3" t="s">
         <v>2</v>
       </c>
@@ -774,36 +774,36 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="18"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="4" t="s">
         <v>18</v>
       </c>
@@ -830,20 +830,23 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A9:N9"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="I7:K7"/>
+  <mergeCells count="16">
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="A4:N4"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I5:L5"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>